<commit_message>
fixup! paper c: reclassifying dataset 3 SetFit
</commit_message>
<xml_diff>
--- a/shared_data/paper_a_correlation_matrices_after_pruning.xlsx
+++ b/shared_data/paper_a_correlation_matrices_after_pruning.xlsx
@@ -678,7 +678,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -694,22 +694,32 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>sentence_complexity</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>personal_pronoun_d</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>passive_voice_d</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>interjection_d</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>modal_verb_d</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>discourse_markers_d</t>
         </is>
       </c>
     </row>
@@ -723,103 +733,189 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
+        <v>0.2939859033294212</v>
+      </c>
+      <c r="D2" t="n">
         <v>-0.06672474766691336</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>0.4035961329072622</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>-0.3153996724127018</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>0.3019432252019841</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.2403625567609906</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>personal_pronoun_d</t>
+          <t>sentence_complexity</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.06672474766691336</v>
+        <v>0.2939859033294212</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3795779975692216</v>
+        <v>0.7373785647927182</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.01415982120200794</v>
+        <v>0.5657222839412497</v>
       </c>
       <c r="F3" t="n">
-        <v>0.4135628921474821</v>
+        <v>-0.1532390230953878</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.4999688335256128</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.7786104552505485</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>passive_voice_d</t>
+          <t>personal_pronoun_d</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.4035961329072622</v>
+        <v>-0.06672474766691336</v>
       </c>
       <c r="C4" t="n">
+        <v>0.7373785647927182</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
         <v>0.3795779975692216</v>
       </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>-0.1227941226378256</v>
-      </c>
       <c r="F4" t="n">
-        <v>0.42186840413018</v>
+        <v>-0.01415982120200794</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.4135628921474821</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.7332728826971066</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>interjection_d</t>
+          <t>passive_voice_d</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.3153996724127018</v>
+        <v>0.4035961329072622</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.01415982120200794</v>
+        <v>0.5657222839412497</v>
       </c>
       <c r="D5" t="n">
+        <v>0.3795779975692216</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
         <v>-0.1227941226378256</v>
       </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" t="n">
-        <v>-0.2609126291512586</v>
+      <c r="G5" t="n">
+        <v>0.42186840413018</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.5765897079294763</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
+          <t>interjection_d</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-0.3153996724127018</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-0.1532390230953878</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-0.01415982120200794</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-0.1227941226378256</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-0.2609126291512586</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.002302043467693686</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
           <t>modal_verb_d</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B7" t="n">
         <v>0.3019432252019841</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C7" t="n">
+        <v>0.4999688335256128</v>
+      </c>
+      <c r="D7" t="n">
         <v>0.4135628921474821</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E7" t="n">
         <v>0.42186840413018</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F7" t="n">
         <v>-0.2609126291512586</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.4580457105838001</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>discourse_markers_d</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.2403625567609906</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.7786104552505485</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.7332728826971066</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.5765897079294763</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.002302043467693686</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.4580457105838001</v>
+      </c>
+      <c r="H8" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>